<commit_message>
Update pivot table test file.
The test Load_and_save_pivot_table_with_cache_records_but_missing_source_data
checks that ClosedXML can survive a file that doesn't contain actual source data,
but has only data in cache.

The better representation of PT means the output file is now more correct (shape
is correct, data still missing from cells), though it still misses the values when
opened in Excel. That will be fixed when we have our own engine to project pivot
table to sheet.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithoutSourceData-output.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithoutSourceData-output.xlsx
@@ -148,51 +148,45 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" indent="0" multipleFieldFilters="0">
-  <x:location ref="A3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="2">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="3">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Sold" dataField="1">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-  </x:pivotFields>
-  <x:rowFields count="1">
-    <x:field x="0"/>
-  </x:rowFields>
-  <x:rowItems count="3">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colItems count="1">
-    <x:i i="0">
-      <x:x v="0"/>
-    </x:i>
-  </x:colItems>
-  <x:dataFields count="1">
-    <x:dataField name="Sum of Sold" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-  </x:dataFields>
-  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sold" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>